<commit_message>
test xlx partage 01
</commit_message>
<xml_diff>
--- a/Test/Classeur1.xlsx
+++ b/Test/Classeur1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\00_APS_SWAP_02\APS_DEV_01_ALL\APS_SWAP02\Test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\00_APS_SWAP02_Git\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,6 +15,10 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <customWorkbookViews>
+    <customWorkbookView name="APS_DEV_01 - Affichage personnalisé" guid="{E0E90811-E8E4-41CC-896E-BD3A5834D2B9}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1096" activeSheetId="1"/>
+    <customWorkbookView name="Alexandre Baranger - Affichage personnalisé" guid="{ABA7904C-BDC2-42DE-B7FC-F95BB0ACB22A}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1096" activeSheetId="1"/>
+  </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,9 +28,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Branche Master</t>
+  </si>
+  <si>
+    <t>Test1</t>
   </si>
 </sst>
 </file>
@@ -79,6 +86,44 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{DC32A037-79E2-4FD8-AD43-7F94D8487E6A}" diskRevisions="1" revisionId="1" version="2">
+  <header guid="{F80BE77D-91B1-4173-A945-8F04FD4E651C}" dateTime="2015-03-05T23:15:59" maxSheetId="2" userName="Alexandre Baranger" r:id="rId1">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{DC32A037-79E2-4FD8-AD43-7F94D8487E6A}" dateTime="2015-03-06T00:15:06" maxSheetId="2" userName="APS_DEV_01" r:id="rId2" minRId="1">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+</headers>
+</file>
+
+<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
+</file>
+
+<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1" sId="1">
+    <nc r="B1" t="inlineStr">
+      <is>
+        <t>Test1</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{E0E90811-E8E4-41CC-896E-BD3A5834D2B9}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
+  <userInfo guid="{DC32A037-79E2-4FD8-AD43-7F94D8487E6A}" name="APS_DEV_01" id="-2127931923" dateTime="2015-03-05T23:34:21"/>
+</users>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -344,10 +389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -355,12 +400,25 @@
     <col min="1" max="1" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
+  <customSheetViews>
+    <customSheetView guid="{E0E90811-E8E4-41CC-896E-BD3A5834D2B9}">
+      <selection activeCell="B2" sqref="B2"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{ABA7904C-BDC2-42DE-B7FC-F95BB0ACB22A}">
+      <selection activeCell="A2" sqref="A2"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+  </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
test partage xls 02
</commit_message>
<xml_diff>
--- a/Test/Classeur1.xlsx
+++ b/Test/Classeur1.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\00_APS_SWAP_02\APS_DEV_01_ALL\APS_SWAP02\Test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Integration\APS_SWAP02\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12555" windowHeight="4590"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9165" windowHeight="4590"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <customWorkbookViews>
+    <customWorkbookView name="Alex - Affichage personnalisé" guid="{24A8138D-215C-45AD-B9A6-4FBBAB36F31D}" mergeInterval="0" personalView="1" xWindow="902" yWindow="155" windowWidth="707" windowHeight="655" activeSheetId="1"/>
+  </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,9 +27,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Branche Master</t>
+  </si>
+  <si>
+    <t>test2</t>
   </si>
 </sst>
 </file>
@@ -79,6 +85,43 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{FDD0F222-BDDD-438B-B606-C33C6947F367}" diskRevisions="1" revisionId="1" version="2">
+  <header guid="{0585ED0A-F665-4B42-94A9-C6DA1DB195F7}" dateTime="2015-03-05T23:24:26" maxSheetId="2" userName="Alex" r:id="rId1">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{FDD0F222-BDDD-438B-B606-C33C6947F367}" dateTime="2015-03-06T00:20:44" maxSheetId="2" userName="Alex" r:id="rId2" minRId="1">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+</headers>
+</file>
+
+<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
+</file>
+
+<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1" sId="1">
+    <nc r="C1" t="inlineStr">
+      <is>
+        <t>test2</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
+  <userInfo guid="{FDD0F222-BDDD-438B-B606-C33C6947F367}" name="Alex" id="-875206765" dateTime="2015-03-05T23:24:26"/>
+</users>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -344,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -355,12 +398,21 @@
     <col min="1" max="1" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
+  <customSheetViews>
+    <customSheetView guid="{24A8138D-215C-45AD-B9A6-4FBBAB36F31D}">
+      <selection activeCell="A2" sqref="A2"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+  </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>